<commit_message>
Corrected error with fresa and vaso
</commit_message>
<xml_diff>
--- a/Analysis/pilot00/pilot00_coded_updated.xlsx
+++ b/Analysis/pilot00/pilot00_coded_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\Analysis\pilot00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AD1A94-28F4-46BE-95E7-D54DC24F17F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1450A924-055C-4348-9CCC-6DEC6FAA4B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilot00_coded_updated" sheetId="1" r:id="rId1"/>
@@ -22613,7 +22613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J388"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -35476,7 +35476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected path in Fam
</commit_message>
<xml_diff>
--- a/Analysis/pilot00/pilot00_coded_updated.xlsx
+++ b/Analysis/pilot00/pilot00_coded_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\Analysis\pilot00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1450A924-055C-4348-9CCC-6DEC6FAA4B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A26C640-13AF-4670-8097-4ECC9FB187D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilot00_coded_updated" sheetId="1" r:id="rId1"/>
@@ -22613,7 +22613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J388"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -35192,7 +35192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -35476,7 +35476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>